<commit_message>
sprint 3 header fixed
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Item ID</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>recreate graph with new library</t>
+  </si>
+  <si>
+    <t>Sprint 3 Backlog</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1254,7 +1257,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1269,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>

</xml_diff>

<commit_message>
Finished test results and analysis
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24000" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,12 @@
     <sheet name="Sp3" sheetId="5" r:id="rId4"/>
     <sheet name="Orig" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -108,6 +113,66 @@
   </si>
   <si>
     <t>Current Product Backlog</t>
+  </si>
+  <si>
+    <t>The user wants to only enter the zip code so that the user has minimal data entry.</t>
+  </si>
+  <si>
+    <t>The web application will store the last accessed data for a saved project in case NOAA database is currently lost or unreliable so that there will still be a prediction.</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Integrate parts and display a graph</t>
+  </si>
+  <si>
+    <t>Improve input and output UI</t>
+  </si>
+  <si>
+    <t>validation for zipcode</t>
+  </si>
+  <si>
+    <t>New Total</t>
+  </si>
+  <si>
+    <t>As a customer I want to have a boundary for the input of the concrete temperature from 45F to 115F</t>
+  </si>
+  <si>
+    <t>As a customer I want to have 12PM labelled as Noon</t>
+  </si>
+  <si>
+    <t>As a customer I want the tooltips to be displayed near the point on the graph</t>
+  </si>
+  <si>
+    <t>As a customer I want evaporation rates to be rounded to two decimals</t>
+  </si>
+  <si>
+    <t>As a customer I want other people to be included in a project to receive notifications as well</t>
+  </si>
+  <si>
+    <t>As a customer I want low-med-high risk to be displayed over the colors in the graph background</t>
+  </si>
+  <si>
+    <t>As a customer I want to have a page that explains how to use the evaporation rate tool and how it works</t>
+  </si>
+  <si>
+    <t>As a customer I want an indication of what zip code the graph is displaying information about</t>
+  </si>
+  <si>
+    <t>As a customer I want to be able to click a point on the graph to change the variables of the formula</t>
+  </si>
+  <si>
+    <t>As a customer I want to see what concrete temperatures are required to lower the evaporation rate</t>
+  </si>
+  <si>
+    <t>Research new graph libraries</t>
+  </si>
+  <si>
+    <t>recreate graph with new library</t>
+  </si>
+  <si>
+    <t>Sprint 3 Backlog</t>
   </si>
   <si>
     <r>
@@ -121,68 +186,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sprint 2</t>
+      <t>Sprint 3 output</t>
     </r>
-  </si>
-  <si>
-    <t>The user wants to only enter the zip code so that the user has minimal data entry.</t>
-  </si>
-  <si>
-    <t>The web application will store the last accessed data for a saved project in case NOAA database is currently lost or unreliable so that there will still be a prediction.</t>
-  </si>
-  <si>
-    <t>Added</t>
-  </si>
-  <si>
-    <t>Integrate parts and display a graph</t>
-  </si>
-  <si>
-    <t>Improve input and output UI</t>
-  </si>
-  <si>
-    <t>validation for zipcode</t>
-  </si>
-  <si>
-    <t>New Total</t>
-  </si>
-  <si>
-    <t>As a customer I want to have a boundary for the input of the concrete temperature from 45F to 115F</t>
-  </si>
-  <si>
-    <t>As a customer I want to have 12PM labelled as Noon</t>
-  </si>
-  <si>
-    <t>As a customer I want the tooltips to be displayed near the point on the graph</t>
-  </si>
-  <si>
-    <t>As a customer I want evaporation rates to be rounded to two decimals</t>
-  </si>
-  <si>
-    <t>As a customer I want other people to be included in a project to receive notifications as well</t>
-  </si>
-  <si>
-    <t>As a customer I want low-med-high risk to be displayed over the colors in the graph background</t>
-  </si>
-  <si>
-    <t>As a customer I want to have a page that explains how to use the evaporation rate tool and how it works</t>
-  </si>
-  <si>
-    <t>As a customer I want an indication of what zip code the graph is displaying information about</t>
-  </si>
-  <si>
-    <t>As a customer I want to be able to click a point on the graph to change the variables of the formula</t>
-  </si>
-  <si>
-    <t>As a customer I want to see what concrete temperatures are required to lower the evaporation rate</t>
-  </si>
-  <si>
-    <t>Research new graph libraries</t>
-  </si>
-  <si>
-    <t>recreate graph with new library</t>
-  </si>
-  <si>
-    <t>Sprint 3 Backlog</t>
   </si>
 </sst>
 </file>
@@ -735,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -745,28 +750,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="72.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.25" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -794,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -808,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -822,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="42">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -836,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="42">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -850,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="42">
       <c r="A8" s="1">
         <v>13</v>
       </c>
@@ -864,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="42">
       <c r="A9" s="1">
         <v>14</v>
       </c>
@@ -878,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28">
       <c r="A10" s="5">
         <v>16</v>
       </c>
@@ -892,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="1">
         <v>17</v>
       </c>
@@ -906,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -914,13 +919,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -934,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28">
       <c r="A14" s="1">
         <v>22</v>
       </c>
@@ -942,13 +947,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -956,13 +961,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="5">
         <v>28</v>
       </c>
@@ -970,13 +975,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="C17" s="12" t="s">
         <v>23</v>
       </c>
@@ -985,7 +990,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
@@ -997,6 +1002,11 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1008,14 +1018,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1033,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1051,7 +1061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1065,24 +1075,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="26"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1097,6 +1107,11 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1108,15 +1123,15 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="25" t="s">
         <v>25</v>
       </c>
@@ -1124,7 +1139,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -1166,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -1180,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28">
       <c r="A6" s="5">
         <v>8</v>
       </c>
@@ -1194,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1203,40 +1218,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="D13" s="18">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="D14" s="18"/>
     </row>
   </sheetData>
@@ -1245,10 +1260,15 @@
     <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1256,26 +1276,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28">
       <c r="A3" s="5">
         <v>12</v>
       </c>
@@ -1303,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="42">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -1317,7 +1337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="5">
         <v>18</v>
       </c>
@@ -1331,7 +1351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>21</v>
       </c>
@@ -1345,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>23</v>
       </c>
@@ -1353,13 +1373,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
         <v>24</v>
       </c>
@@ -1367,13 +1387,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>25</v>
       </c>
@@ -1381,13 +1401,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28">
       <c r="A10" s="4">
         <v>27</v>
       </c>
@@ -1395,13 +1415,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="4">
         <v>29</v>
       </c>
@@ -1409,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28">
       <c r="A12" s="5">
         <v>30</v>
       </c>
@@ -1423,13 +1443,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="22">
         <v>31</v>
       </c>
@@ -1437,40 +1457,40 @@
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="26"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="26"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D16" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
       <c r="D17" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="19">
         <f>SUM(D3:D17)</f>
@@ -1483,6 +1503,11 @@
     <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1494,15 +1519,15 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="94.83203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1530,7 +1555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1541,7 +1566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,13 +1574,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1569,7 +1594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1583,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1597,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1611,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1625,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1639,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1653,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="42">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1667,7 +1692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1681,7 +1706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1695,7 +1720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1709,7 +1734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1723,7 +1748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1737,7 +1762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1751,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1765,7 +1790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1773,13 +1798,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1793,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1807,7 +1832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="C23" s="12" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
fixed status report and graphs
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="25605" windowHeight="14415"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sp3" sheetId="5" r:id="rId4"/>
     <sheet name="Orig" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -740,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -754,14 +754,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="72.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" customHeight="1">
+    <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
@@ -771,7 +771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -799,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -813,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -841,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -855,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="42">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>13</v>
       </c>
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>14</v>
       </c>
@@ -883,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>16</v>
       </c>
@@ -897,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>17</v>
       </c>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -925,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -939,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>22</v>
       </c>
@@ -953,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -967,7 +967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>28</v>
       </c>
@@ -981,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" s="12" t="s">
         <v>23</v>
       </c>
@@ -990,7 +990,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
@@ -1018,14 +1018,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1075,16 +1075,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="26"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1120,18 +1120,18 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>25</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>8</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1218,13 +1218,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>34</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>35</v>
       </c>
@@ -1240,10 +1240,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
     </row>
   </sheetData>
@@ -1277,17 +1277,17 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>49</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>12</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>18</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>21</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>23</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>24</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>25</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>27</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>29</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>30</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>31</v>
       </c>
@@ -1463,13 +1463,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="26"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>47</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>48</v>
       </c>
@@ -1485,10 +1485,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1515,19 +1515,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94.83203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="94.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="42">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="12" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Update backlog and sprint output
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="-15" windowWidth="7200" windowHeight="13005" activeTab="5"/>
+    <workbookView xWindow="12800" yWindow="-20" windowWidth="12800" windowHeight="14480" tabRatio="697" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Sp3" sheetId="5" r:id="rId5"/>
     <sheet name="Sp4" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>Item ID</t>
   </si>
@@ -192,6 +192,24 @@
   </si>
   <si>
     <t>Sprint 4 Backlog</t>
+  </si>
+  <si>
+    <t>Create Projects Page</t>
+  </si>
+  <si>
+    <t>Create Account Page</t>
+  </si>
+  <si>
+    <t>Various formatting fixes</t>
+  </si>
+  <si>
+    <t>Change time to account for timezones</t>
+  </si>
+  <si>
+    <t>Change windspeed functionality</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -283,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +373,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -363,6 +384,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,7 +771,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -761,24 +785,24 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="72.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4" ht="26.25" customHeight="1">
+      <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -806,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="42">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -820,7 +844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="42">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -834,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="42">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -848,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="1">
         <v>20</v>
       </c>
@@ -862,7 +886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>26</v>
       </c>
@@ -876,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
@@ -885,7 +909,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
@@ -913,15 +937,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="94.83203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -935,7 +959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -949,7 +973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -960,7 +984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -974,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -988,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1002,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1016,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1030,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1044,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1058,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1072,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="42">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1086,7 +1110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1100,7 +1124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1128,7 +1152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1142,7 +1166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1156,7 +1180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1170,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1184,7 +1208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1198,7 +1222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1212,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1226,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="C23" s="12" t="s">
         <v>23</v>
       </c>
@@ -1257,22 +1281,22 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28">
+      <c r="A1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1310,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1300,7 +1324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1314,16 +1338,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="27"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="28"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="C7" t="s">
         <v>33</v>
       </c>
@@ -1331,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1362,23 +1386,23 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28">
+      <c r="A1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1406,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -1420,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -1434,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28">
       <c r="A6" s="5">
         <v>8</v>
       </c>
@@ -1448,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1457,13 +1481,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="28"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="C10" t="s">
         <v>34</v>
       </c>
@@ -1471,7 +1495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="C11" t="s">
         <v>35</v>
       </c>
@@ -1479,10 +1503,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
@@ -1490,7 +1514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="D14" s="18"/>
     </row>
   </sheetData>
@@ -1519,22 +1543,22 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28">
+      <c r="A1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28">
       <c r="A3" s="5">
         <v>12</v>
       </c>
@@ -1562,7 +1586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="42">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -1576,7 +1600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="5">
         <v>18</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>21</v>
       </c>
@@ -1604,7 +1628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>23</v>
       </c>
@@ -1618,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
         <v>24</v>
       </c>
@@ -1632,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>25</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28">
       <c r="A10" s="4">
         <v>27</v>
       </c>
@@ -1660,7 +1684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="4">
         <v>29</v>
       </c>
@@ -1674,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28">
       <c r="A12" s="5">
         <v>30</v>
       </c>
@@ -1688,7 +1712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="22">
         <v>31</v>
       </c>
@@ -1702,13 +1726,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="27"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="C16" t="s">
         <v>47</v>
       </c>
@@ -1716,7 +1740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="C17" t="s">
         <v>48</v>
       </c>
@@ -1724,10 +1748,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="C19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1752,28 +1776,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28">
+      <c r="A1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -1801,7 +1825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28">
       <c r="A4" s="5">
         <v>7</v>
       </c>
@@ -1815,7 +1839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="4">
         <v>9</v>
       </c>
@@ -1829,13 +1853,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="20"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="4">
         <v>16</v>
       </c>
@@ -1849,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="5">
         <v>17</v>
       </c>
@@ -1863,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="4">
         <v>19</v>
       </c>
@@ -1877,7 +1901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28">
       <c r="A10" s="4">
         <v>22</v>
       </c>
@@ -1891,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="22">
         <v>28</v>
       </c>
@@ -1905,26 +1929,72 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="D12" s="24"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="9" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="C14" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="29"/>
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="24">
-        <f>SUM(D3:D13)</f>
-        <v>39</v>
+      <c r="D20" s="24">
+        <f>SUM(D3:D18)</f>
+        <v>61.5</v>
       </c>
     </row>
   </sheetData>
@@ -1933,5 +2003,11 @@
     <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated sprint 4 documents
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="-20" windowWidth="12800" windowHeight="14480" tabRatio="697" activeTab="5"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14480" tabRatio="697"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t>Item ID</t>
   </si>
@@ -210,6 +210,39 @@
   </si>
   <si>
     <t>Research</t>
+  </si>
+  <si>
+    <t>Move files to server</t>
+  </si>
+  <si>
+    <t>Add metric button to graph page</t>
+  </si>
+  <si>
+    <t>Add tooltips to buttons</t>
+  </si>
+  <si>
+    <t>Reset button only appears after a series has been added</t>
+  </si>
+  <si>
+    <t>Add series based on user input of concrete temperature and wind speed</t>
+  </si>
+  <si>
+    <t>Add local time for zip code instead of time zone</t>
+  </si>
+  <si>
+    <t>Add sticky notes</t>
+  </si>
+  <si>
+    <t>The system checks once a day for updated weather predictions</t>
+  </si>
+  <si>
+    <t>Projects get deleted after one month of when the graph was created. After a week the proejct will have an option to re update the graph for the next week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We will create notifications for various zip codes and see how much the prediction changes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamically assign height of graph </t>
   </si>
 </sst>
 </file>
@@ -301,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,6 +409,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -385,7 +421,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -472,8 +511,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D20"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A1:A23"/>
   </sortState>
@@ -771,7 +810,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -779,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -793,11 +832,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="14" t="s">
         <v>50</v>
       </c>
@@ -887,31 +926,191 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>26</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="12" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="30">
+        <v>27</v>
+      </c>
+      <c r="B10" s="30">
+        <v>1</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="30">
+        <v>28</v>
+      </c>
+      <c r="B11" s="30">
+        <v>2</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="30">
+        <v>29</v>
+      </c>
+      <c r="B12" s="30">
+        <v>2</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="30">
+        <v>30</v>
+      </c>
+      <c r="B13" s="30">
+        <v>2</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="30">
+        <v>31</v>
+      </c>
+      <c r="B14" s="30">
+        <v>3</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="30">
+        <v>32</v>
+      </c>
+      <c r="B15" s="30">
+        <v>1</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="30">
+        <v>33</v>
+      </c>
+      <c r="B16" s="30">
+        <v>3</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="30">
+        <v>34</v>
+      </c>
+      <c r="B17" s="30">
+        <v>2</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="30">
+        <v>35</v>
+      </c>
+      <c r="B18" s="30">
+        <v>1</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28">
+      <c r="A19" s="30">
+        <v>36</v>
+      </c>
+      <c r="B19" s="30">
+        <v>2</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="30">
+        <v>37</v>
+      </c>
+      <c r="B20" s="30">
+        <v>1</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D21" s="1">
         <f>SUM(Table13[Estimated remaining (person-hours)])</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1289,12 +1488,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -1342,10 +1541,10 @@
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="29"/>
     </row>
     <row r="7" spans="1:4">
       <c r="C7" t="s">
@@ -1395,12 +1594,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -1482,10 +1681,10 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="29"/>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" t="s">
@@ -1551,12 +1750,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -1727,10 +1926,10 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="29"/>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" t="s">
@@ -1778,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1790,12 +1989,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
@@ -1933,11 +2132,11 @@
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="26" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="24">
@@ -1945,7 +2144,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="26" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="24">
@@ -1953,7 +2152,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="26" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="25">
@@ -1961,7 +2160,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="25">
@@ -1969,7 +2168,7 @@
       </c>
     </row>
     <row r="17" spans="3:4">
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="26" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="25">
@@ -1977,7 +2176,7 @@
       </c>
     </row>
     <row r="18" spans="3:4">
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="26" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="25">
@@ -1985,7 +2184,7 @@
       </c>
     </row>
     <row r="19" spans="3:4">
-      <c r="C19" s="29"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="25"/>
     </row>
     <row r="20" spans="3:4">

</xml_diff>

<commit_message>
Completed Sprint 5 prep
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14480" tabRatio="697"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480" tabRatio="844"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sp2" sheetId="4" r:id="rId4"/>
     <sheet name="Sp3" sheetId="5" r:id="rId5"/>
     <sheet name="Sp4" sheetId="7" r:id="rId6"/>
+    <sheet name="Sp5" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Item ID</t>
   </si>
@@ -244,12 +245,30 @@
   <si>
     <t xml:space="preserve">Dynamically assign height of graph </t>
   </si>
+  <si>
+    <t>Sprint 5 Backlog</t>
+  </si>
+  <si>
+    <t>Finish Database interaction classes</t>
+  </si>
+  <si>
+    <t>Added:</t>
+  </si>
+  <si>
+    <t>x-axis graph formating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing system </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +317,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,8 +353,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -330,11 +377,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,8 +487,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -820,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1117,6 +1199,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1977,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2209,4 +2292,261 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28">
+      <c r="A1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28">
+      <c r="A3" s="32">
+        <v>26</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="34">
+        <v>27</v>
+      </c>
+      <c r="B4" s="34">
+        <v>1</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="32">
+        <v>28</v>
+      </c>
+      <c r="B5" s="32">
+        <v>2</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="34">
+        <v>29</v>
+      </c>
+      <c r="B6" s="34">
+        <v>2</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="32">
+        <v>30</v>
+      </c>
+      <c r="B7" s="32">
+        <v>2</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="34">
+        <v>31</v>
+      </c>
+      <c r="B8" s="34">
+        <v>3</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="32">
+        <v>32</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="34">
+        <v>33</v>
+      </c>
+      <c r="B10" s="34">
+        <v>3</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="32">
+        <v>34</v>
+      </c>
+      <c r="B11" s="32">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="34">
+        <v>35</v>
+      </c>
+      <c r="B12" s="34">
+        <v>1</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28">
+      <c r="A13" s="32">
+        <v>36</v>
+      </c>
+      <c r="B13" s="32">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28">
+      <c r="A14" s="36">
+        <v>37</v>
+      </c>
+      <c r="B14" s="36">
+        <v>1</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="D22">
+        <f>SUM(D3:D19)</f>
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated for status report
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480" tabRatio="844" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14475" tabRatio="844"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Sp4" sheetId="7" r:id="rId6"/>
     <sheet name="Sp5" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -871,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -881,18 +881,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="72.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" customHeight="1">
+    <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>29</v>
       </c>
@@ -902,7 +902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -930,7 +930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -941,10 +941,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -955,10 +955,10 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -969,10 +969,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>20</v>
       </c>
@@ -983,10 +983,10 @@
         <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>35</v>
       </c>
@@ -997,19 +997,19 @@
         <v>64</v>
       </c>
       <c r="D8" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(Table13[Estimated remaining (person-hours)])</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
@@ -1038,15 +1038,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94.83203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="94.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="42">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="12" t="s">
         <v>23</v>
       </c>
@@ -1382,14 +1382,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>27</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1439,16 +1439,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="35"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>33</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1487,15 +1487,15 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>8</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1582,13 +1582,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="35"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>35</v>
       </c>
@@ -1604,10 +1604,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
     </row>
   </sheetData>
@@ -1644,14 +1644,14 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>49</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>12</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>18</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>21</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>23</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>24</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>25</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>27</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>29</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>30</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>31</v>
       </c>
@@ -1827,13 +1827,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="35"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>47</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>48</v>
       </c>
@@ -1849,10 +1849,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1883,14 +1883,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>51</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>7</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>9</v>
       </c>
@@ -1954,13 +1954,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="20"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="28">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>16</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>17</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>19</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>22</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>28</v>
       </c>
@@ -2030,10 +2030,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="24"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>32</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="26" t="s">
         <v>53</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="26" t="s">
         <v>54</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="26" t="s">
         <v>55</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="26" t="s">
         <v>56</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="26" t="s">
         <v>57</v>
       </c>
@@ -2085,11 +2085,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="26"/>
       <c r="D19" s="25"/>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="9" t="s">
         <v>36</v>
       </c>
@@ -2117,18 +2117,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>66</v>
       </c>
@@ -2136,7 +2136,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>26</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>28</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>29</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>30</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>31</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>32</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>33</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>34</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>36</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>69</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>71</v>
       </c>
@@ -2303,12 +2303,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19">
         <f>SUM(D3:D16)</f>
         <v>48</v>

</xml_diff>

<commit_message>
updated for sprint 5
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Sp3" sheetId="5" r:id="rId5"/>
     <sheet name="Sp4" sheetId="7" r:id="rId6"/>
     <sheet name="Sp5" sheetId="9" r:id="rId7"/>
+    <sheet name="Sp6" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Item ID</t>
   </si>
@@ -175,6 +176,72 @@
   </si>
   <si>
     <t>Sprint 3 Backlog</t>
+  </si>
+  <si>
+    <t>Sprint 4 Backlog</t>
+  </si>
+  <si>
+    <t>Create Projects Page</t>
+  </si>
+  <si>
+    <t>Create Account Page</t>
+  </si>
+  <si>
+    <t>Various formatting fixes</t>
+  </si>
+  <si>
+    <t>Change time to account for timezones</t>
+  </si>
+  <si>
+    <t>Change windspeed functionality</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Add metric button to graph page</t>
+  </si>
+  <si>
+    <t>Add tooltips to buttons</t>
+  </si>
+  <si>
+    <t>Reset button only appears after a series has been added</t>
+  </si>
+  <si>
+    <t>Add series based on user input of concrete temperature and wind speed</t>
+  </si>
+  <si>
+    <t>Add local time for zip code instead of time zone</t>
+  </si>
+  <si>
+    <t>Add sticky notes</t>
+  </si>
+  <si>
+    <t>The system checks once a day for updated weather predictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamically assign height of graph </t>
+  </si>
+  <si>
+    <t>Sprint 5 Backlog</t>
+  </si>
+  <si>
+    <t>Finish Database interaction classes</t>
+  </si>
+  <si>
+    <t>Added:</t>
+  </si>
+  <si>
+    <t>x-axis graph formating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing system </t>
+  </si>
+  <si>
+    <t>Projects get deleted after one month of when the graph was created. After a week the project will have an option to r- update the graph for the next week</t>
   </si>
   <si>
     <r>
@@ -188,74 +255,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sprint 4</t>
+      <t>Sprint 5</t>
     </r>
   </si>
   <si>
-    <t>Sprint 4 Backlog</t>
-  </si>
-  <si>
-    <t>Create Projects Page</t>
-  </si>
-  <si>
-    <t>Create Account Page</t>
-  </si>
-  <si>
-    <t>Various formatting fixes</t>
-  </si>
-  <si>
-    <t>Change time to account for timezones</t>
-  </si>
-  <si>
-    <t>Change windspeed functionality</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Add metric button to graph page</t>
-  </si>
-  <si>
-    <t>Add tooltips to buttons</t>
-  </si>
-  <si>
-    <t>Reset button only appears after a series has been added</t>
-  </si>
-  <si>
-    <t>Add series based on user input of concrete temperature and wind speed</t>
-  </si>
-  <si>
-    <t>Add local time for zip code instead of time zone</t>
-  </si>
-  <si>
-    <t>Add sticky notes</t>
-  </si>
-  <si>
-    <t>The system checks once a day for updated weather predictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dynamically assign height of graph </t>
-  </si>
-  <si>
-    <t>Sprint 5 Backlog</t>
-  </si>
-  <si>
-    <t>Finish Database interaction classes</t>
-  </si>
-  <si>
-    <t>Added:</t>
-  </si>
-  <si>
-    <t>x-axis graph formating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing system </t>
-  </si>
-  <si>
-    <t>Projects get deleted after one month of when the graph was created. After a week the project will have an option to r- update the graph for the next week</t>
+    <t>Sprint 6 Backlog</t>
   </si>
 </sst>
 </file>
@@ -457,12 +461,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,6 +481,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -493,6 +497,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -526,13 +537,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -572,32 +576,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
   <autoFilter ref="A2:D8"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
-    <tableColumn id="2" name="Priority" dataDxfId="8"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="10"/>
+    <tableColumn id="2" name="Priority" dataDxfId="9"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:D22"/>
   <sortState ref="A2:D23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
-    <tableColumn id="2" name="Priority" dataDxfId="2"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="5"/>
+    <tableColumn id="2" name="Priority" dataDxfId="4"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="3"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -882,7 +886,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,13 +897,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="14" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,97 +920,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
-        <v>35</v>
-      </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="27">
-        <v>6</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(Table13[Estimated remaining (person-hours)])</f>
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1390,12 +1310,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1443,10 +1363,10 @@
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -1496,12 +1416,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1583,10 +1503,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -1652,12 +1572,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1828,10 +1748,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="33"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -1891,12 +1811,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="A1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2034,12 +1954,12 @@
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="24">
         <v>2</v>
@@ -2047,7 +1967,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="24">
         <v>2</v>
@@ -2055,7 +1975,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="25">
         <v>10</v>
@@ -2063,7 +1983,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="25">
         <v>2</v>
@@ -2071,7 +1991,7 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="25">
         <v>4.5</v>
@@ -2079,7 +1999,7 @@
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="25">
         <v>2</v>
@@ -2118,7 +2038,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,12 +2049,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="A1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2151,137 +2071,137 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="27">
         <v>26</v>
       </c>
-      <c r="B3" s="29">
-        <v>2</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="27">
+        <v>2</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="A4" s="27">
         <v>28</v>
       </c>
-      <c r="B4" s="29">
-        <v>2</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+      <c r="A5" s="29">
         <v>29</v>
       </c>
-      <c r="B5" s="31">
-        <v>2</v>
-      </c>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="29">
+        <v>2</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>30</v>
+      </c>
+      <c r="B6" s="27">
+        <v>2</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
-        <v>30</v>
-      </c>
-      <c r="B6" s="29">
-        <v>2</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>31</v>
+      </c>
+      <c r="B7" s="29">
+        <v>3</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>31</v>
-      </c>
-      <c r="B7" s="31">
-        <v>3</v>
-      </c>
-      <c r="C7" s="32" t="s">
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>32</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>32</v>
-      </c>
-      <c r="B8" s="29">
-        <v>1</v>
-      </c>
-      <c r="C8" s="30" t="s">
+      <c r="D8" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>33</v>
+      </c>
+      <c r="B9" s="29">
+        <v>3</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>33</v>
-      </c>
-      <c r="B9" s="31">
-        <v>3</v>
-      </c>
-      <c r="C9" s="32" t="s">
+      <c r="D9" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>34</v>
+      </c>
+      <c r="B10" s="27">
+        <v>2</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
-        <v>34</v>
-      </c>
-      <c r="B10" s="29">
-        <v>2</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="29">
+      <c r="D10" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="27">
         <v>36</v>
       </c>
-      <c r="B11" s="29">
-        <v>2</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="B11" s="27">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>15</v>
@@ -2289,7 +2209,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2297,7 +2217,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2305,7 +2225,7 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
@@ -2326,4 +2246,148 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>35</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>SUM(D3:D8)</f>
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated for use on siue server
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14475" tabRatio="844"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14475" tabRatio="844" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Item ID</t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>Add sticky notes</t>
-  </si>
-  <si>
-    <t>The system checks once a day for updated weather predictions</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamically assign height of graph </t>
@@ -260,6 +257,24 @@
   </si>
   <si>
     <t>Sprint 6 Backlog</t>
+  </si>
+  <si>
+    <t>I want multiple colors for series to add to my project and easy to use tooltips for multiple series</t>
+  </si>
+  <si>
+    <t>I want the graph to load in no longer than 5 seconds</t>
+  </si>
+  <si>
+    <t>I want the application to work the same on ie, firefox, chrome, and safari</t>
+  </si>
+  <si>
+    <t>As an administrator I want to be able to drop the databases if there is an error</t>
+  </si>
+  <si>
+    <t>As a user I want to have the application to be easy to use</t>
+  </si>
+  <si>
+    <t>As a user I want the project to be on the siue virtual server</t>
   </si>
 </sst>
 </file>
@@ -383,7 +398,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,6 +488,15 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,12 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -497,13 +515,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -537,6 +548,13 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -576,32 +594,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:D8"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="10"/>
-    <tableColumn id="2" name="Priority" dataDxfId="9"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="8"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
+    <tableColumn id="2" name="Priority" dataDxfId="8"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D22"/>
   <sortState ref="A2:D23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Priority" dataDxfId="4"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="3"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="2"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
+    <tableColumn id="2" name="Priority" dataDxfId="2"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -897,13 +915,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1310,12 +1328,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1363,10 +1381,10 @@
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="36"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -1416,12 +1434,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1503,10 +1521,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -1561,7 +1579,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,12 +1590,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1748,10 +1766,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="36"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -1800,7 +1818,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,12 +1829,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1954,10 +1972,10 @@
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="26" t="s">
         <v>51</v>
       </c>
@@ -2038,7 +2056,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,12 +2067,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="A1" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2092,7 +2110,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="27">
         <v>1</v>
@@ -2190,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="27">
         <v>3</v>
@@ -2198,10 +2216,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>15</v>
@@ -2209,7 +2227,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2217,7 +2235,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2225,7 +2243,7 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
@@ -2250,26 +2268,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="A1" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2296,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2310,35 +2328,35 @@
         <v>5</v>
       </c>
       <c r="D4" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8</v>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2355,32 +2373,118 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
-        <v>35</v>
-      </c>
-      <c r="B8" s="34">
-        <v>1</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="34">
-        <v>6</v>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>26</v>
+      </c>
+      <c r="B8" s="27">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4">
+        <v>4</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
+      <c r="A10" s="31">
+        <v>37</v>
+      </c>
+      <c r="B10" s="31">
+        <v>1</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="31">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f>SUM(D3:D8)</f>
+      <c r="A11" s="31">
+        <v>38</v>
+      </c>
+      <c r="B11" s="31">
+        <v>1</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>39</v>
+      </c>
+      <c r="B12" s="31">
+        <v>1</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>40</v>
+      </c>
+      <c r="B13" s="31">
+        <v>1</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>41</v>
+      </c>
+      <c r="B14" s="31">
+        <v>1</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>SUM(D3:D14)</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for sprint 6
</commit_message>
<xml_diff>
--- a/Management/Backlog.xlsx
+++ b/Management/Backlog.xlsx
@@ -241,6 +241,27 @@
     <t>Projects get deleted after one month of when the graph was created. After a week the project will have an option to r- update the graph for the next week</t>
   </si>
   <si>
+    <t>Sprint 6 Backlog</t>
+  </si>
+  <si>
+    <t>I want multiple colors for series to add to my project and easy to use tooltips for multiple series</t>
+  </si>
+  <si>
+    <t>I want the graph to load in no longer than 5 seconds</t>
+  </si>
+  <si>
+    <t>I want the application to work the same on ie, firefox, chrome, and safari</t>
+  </si>
+  <si>
+    <t>As an administrator I want to be able to drop the databases if there is an error</t>
+  </si>
+  <si>
+    <t>As a user I want to have the application to be easy to use</t>
+  </si>
+  <si>
+    <t>As a user I want the project to be on the siue virtual server</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">As Of: </t>
     </r>
@@ -252,29 +273,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sprint 5</t>
+      <t>Sprint 6</t>
     </r>
-  </si>
-  <si>
-    <t>Sprint 6 Backlog</t>
-  </si>
-  <si>
-    <t>I want multiple colors for series to add to my project and easy to use tooltips for multiple series</t>
-  </si>
-  <si>
-    <t>I want the graph to load in no longer than 5 seconds</t>
-  </si>
-  <si>
-    <t>I want the application to work the same on ie, firefox, chrome, and safari</t>
-  </si>
-  <si>
-    <t>As an administrator I want to be able to drop the databases if there is an error</t>
-  </si>
-  <si>
-    <t>As a user I want to have the application to be easy to use</t>
-  </si>
-  <si>
-    <t>As a user I want the project to be on the siue virtual server</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -921,7 +921,7 @@
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
       <c r="D1" s="14" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B16" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -2283,7 +2283,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -2395,7 +2395,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -2409,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="31">
         <v>2</v>
@@ -2423,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="31">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="31">
         <v>1</v>
@@ -2451,7 +2451,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="31">
         <v>2</v>
@@ -2465,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="31">
         <v>2</v>

</xml_diff>